<commit_message>
Sin el script de correlación
</commit_message>
<xml_diff>
--- a/datos1.xlsx
+++ b/datos1.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CFD2FF0-112E-42EC-8973-B46C0DA6F7E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CFD2FF0-112E-42EC-8973-B46C0DA6F7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B75C5BE-C44D-450E-8614-D8762847364A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,7 +41,16 @@
     <t>Fecha</t>
   </si>
   <si>
+    <t>Linea</t>
+  </si>
+  <si>
+    <t>Tratamiento</t>
+  </si>
+  <si>
     <t>Repetición</t>
+  </si>
+  <si>
+    <t>Textura</t>
   </si>
   <si>
     <t>SPAD</t>
@@ -42,19 +62,10 @@
     <t>Medición</t>
   </si>
   <si>
-    <t>Tratamiento</t>
-  </si>
-  <si>
-    <t>Linea</t>
+    <t>AV</t>
   </si>
   <si>
     <t>RA</t>
-  </si>
-  <si>
-    <t>Textura</t>
-  </si>
-  <si>
-    <t>AV</t>
   </si>
   <si>
     <t>VA</t>
@@ -91,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,34 +229,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -256,60 +267,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -532,7 +489,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -555,6 +512,60 @@
         </top>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -569,27 +580,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05BA2E7D-E62E-4B9C-906C-46F03BC897B6}" name="Tabla3" displayName="Tabla3" ref="A1:H97" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05BA2E7D-E62E-4B9C-906C-46F03BC897B6}" name="Tabla3" displayName="Tabla3" ref="A1:H97" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:H97" xr:uid="{F34713B2-9C0F-46CF-9387-124409E6314D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H97">
     <sortCondition ref="H1:H97"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A50326C3-9017-4379-B69E-2277C6B862E7}" name="Fecha" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{9ADA6F0D-0FE5-4A51-A123-B514CD233830}" name="Linea" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B244293D-37ED-4AC8-B623-5C59A0FA2F1E}" name="Tratamiento" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{51CA310B-BA3E-4659-BBAB-9F6DD98441F5}" name="Repetición" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{4064E715-5E4A-4171-8F99-2CED46162F2B}" name="Textura" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4516A926-3883-486E-8F56-04F0F615CDCD}" name="SPAD" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{1A862813-268A-4823-B5D2-E8CB2DD523C1}" name="ALTURA" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{636BD3B6-96DE-4FE5-9D2D-A83B373787CA}" name="Medición" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A50326C3-9017-4379-B69E-2277C6B862E7}" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{9ADA6F0D-0FE5-4A51-A123-B514CD233830}" name="Linea" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B244293D-37ED-4AC8-B623-5C59A0FA2F1E}" name="Tratamiento" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{51CA310B-BA3E-4659-BBAB-9F6DD98441F5}" name="Repetición" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4064E715-5E4A-4171-8F99-2CED46162F2B}" name="Textura" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4516A926-3883-486E-8F56-04F0F615CDCD}" name="SPAD" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1A862813-268A-4823-B5D2-E8CB2DD523C1}" name="ALTURA" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{636BD3B6-96DE-4FE5-9D2D-A83B373787CA}" name="Medición" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -891,47 +902,48 @@
       <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="2">
         <v>45826</v>
       </c>
@@ -939,7 +951,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
@@ -958,7 +970,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="9">
         <v>45826</v>
       </c>
@@ -966,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -985,7 +997,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="2">
         <v>45826</v>
       </c>
@@ -993,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>4</v>
@@ -1012,7 +1024,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="9">
         <v>45826</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -1039,7 +1051,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="2">
         <v>45826</v>
       </c>
@@ -1047,7 +1059,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -1066,7 +1078,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="9">
         <v>45826</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -1093,7 +1105,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>45826</v>
       </c>
@@ -1120,7 +1132,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="9">
         <v>45826</v>
       </c>
@@ -1147,7 +1159,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
         <v>45826</v>
       </c>
@@ -1174,7 +1186,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="9">
         <v>45826</v>
       </c>
@@ -1201,7 +1213,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="2">
         <v>45826</v>
       </c>
@@ -1228,7 +1240,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="9">
         <v>45826</v>
       </c>
@@ -1255,7 +1267,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="2">
         <v>45826</v>
       </c>
@@ -1282,7 +1294,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="9">
         <v>45826</v>
       </c>
@@ -1309,7 +1321,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="2">
         <v>45826</v>
       </c>
@@ -1336,7 +1348,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="9">
         <v>45826</v>
       </c>
@@ -1363,7 +1375,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>45826</v>
       </c>
@@ -1390,7 +1402,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="9">
         <v>45826</v>
       </c>
@@ -1417,7 +1429,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>45826</v>
       </c>
@@ -1444,7 +1456,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="9">
         <v>45826</v>
       </c>
@@ -1471,7 +1483,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>45826</v>
       </c>
@@ -1498,7 +1510,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="9">
         <v>45826</v>
       </c>
@@ -1525,7 +1537,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>45826</v>
       </c>
@@ -1552,7 +1564,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="9">
         <v>45826</v>
       </c>
@@ -1579,7 +1591,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>45826</v>
       </c>
@@ -1606,7 +1618,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="9">
         <v>45826</v>
       </c>
@@ -1633,7 +1645,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>45826</v>
       </c>
@@ -1641,7 +1653,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3">
         <v>4</v>
@@ -1660,7 +1672,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="9">
         <v>45826</v>
       </c>
@@ -1668,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D29" s="5">
         <v>4</v>
@@ -1687,7 +1699,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>45826</v>
       </c>
@@ -1714,7 +1726,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="9">
         <v>45826</v>
       </c>
@@ -1741,7 +1753,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>45826</v>
       </c>
@@ -1768,7 +1780,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9">
       <c r="A33" s="9">
         <v>45826</v>
       </c>
@@ -1795,7 +1807,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34" s="2">
         <v>45826</v>
       </c>
@@ -1822,7 +1834,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9">
       <c r="A35" s="9">
         <v>45826</v>
       </c>
@@ -1849,7 +1861,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9">
       <c r="A36" s="2">
         <v>45826</v>
       </c>
@@ -1876,7 +1888,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9">
       <c r="A37" s="9">
         <v>45826</v>
       </c>
@@ -1903,7 +1915,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9">
       <c r="A38" s="2">
         <v>45826</v>
       </c>
@@ -1930,7 +1942,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9">
       <c r="A39" s="9">
         <v>45826</v>
       </c>
@@ -1957,7 +1969,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9">
       <c r="A40" s="2">
         <v>45826</v>
       </c>
@@ -1984,7 +1996,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9">
       <c r="A41" s="9">
         <v>45826</v>
       </c>
@@ -2011,7 +2023,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9">
       <c r="A42" s="2">
         <v>45826</v>
       </c>
@@ -2038,7 +2050,7 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9">
       <c r="A43" s="9">
         <v>45826</v>
       </c>
@@ -2065,7 +2077,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9">
       <c r="A44" s="2">
         <v>45826</v>
       </c>
@@ -2092,7 +2104,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9">
       <c r="A45" s="9">
         <v>45826</v>
       </c>
@@ -2119,7 +2131,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9">
       <c r="A46" s="2">
         <v>45826</v>
       </c>
@@ -2146,7 +2158,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9">
       <c r="A47" s="9">
         <v>45826</v>
       </c>
@@ -2173,7 +2185,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9">
       <c r="A48" s="2">
         <v>45826</v>
       </c>
@@ -2181,7 +2193,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" s="3">
         <v>2</v>
@@ -2200,7 +2212,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9">
       <c r="A49" s="9">
         <v>45826</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49" s="5">
         <v>2</v>
@@ -2227,7 +2239,7 @@
       </c>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>45826</v>
       </c>
@@ -2235,7 +2247,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
@@ -2254,7 +2266,7 @@
       </c>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9">
       <c r="A51" s="9">
         <v>45826</v>
       </c>
@@ -2262,7 +2274,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51" s="5">
         <v>1</v>
@@ -2281,7 +2293,7 @@
       </c>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9">
       <c r="A52" s="2">
         <v>45826</v>
       </c>
@@ -2308,7 +2320,7 @@
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9">
       <c r="A53" s="9">
         <v>45826</v>
       </c>
@@ -2335,7 +2347,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>45826</v>
       </c>
@@ -2362,7 +2374,7 @@
       </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9">
       <c r="A55" s="9">
         <v>45826</v>
       </c>
@@ -2389,7 +2401,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9">
       <c r="A56" s="2">
         <v>45826</v>
       </c>
@@ -2416,7 +2428,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9">
       <c r="A57" s="9">
         <v>45826</v>
       </c>
@@ -2443,7 +2455,7 @@
       </c>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9">
       <c r="A58" s="2">
         <v>45826</v>
       </c>
@@ -2470,7 +2482,7 @@
       </c>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9">
       <c r="A59" s="9">
         <v>45826</v>
       </c>
@@ -2497,7 +2509,7 @@
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9">
       <c r="A60" s="2">
         <v>45826</v>
       </c>
@@ -2524,7 +2536,7 @@
       </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9">
       <c r="A61" s="9">
         <v>45826</v>
       </c>
@@ -2551,7 +2563,7 @@
       </c>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9">
       <c r="A62" s="2">
         <v>45826</v>
       </c>
@@ -2578,7 +2590,7 @@
       </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9">
       <c r="A63" s="9">
         <v>45826</v>
       </c>
@@ -2605,7 +2617,7 @@
       </c>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9">
       <c r="A64" s="2">
         <v>45826</v>
       </c>
@@ -2632,7 +2644,7 @@
       </c>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9">
       <c r="A65" s="9">
         <v>45826</v>
       </c>
@@ -2659,7 +2671,7 @@
       </c>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9">
       <c r="A66" s="2">
         <v>45826</v>
       </c>
@@ -2686,7 +2698,7 @@
       </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9">
       <c r="A67" s="9">
         <v>45826</v>
       </c>
@@ -2713,7 +2725,7 @@
       </c>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9">
       <c r="A68" s="2">
         <v>45826</v>
       </c>
@@ -2740,7 +2752,7 @@
       </c>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9">
       <c r="A69" s="9">
         <v>45826</v>
       </c>
@@ -2767,7 +2779,7 @@
       </c>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9">
       <c r="A70" s="2">
         <v>45826</v>
       </c>
@@ -2794,7 +2806,7 @@
       </c>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9">
       <c r="A71" s="9">
         <v>45826</v>
       </c>
@@ -2821,7 +2833,7 @@
       </c>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9">
       <c r="A72" s="2">
         <v>45826</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>15</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D72" s="3">
         <v>2</v>
@@ -2848,7 +2860,7 @@
       </c>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9">
       <c r="A73" s="9">
         <v>45826</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>15</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D73" s="5">
         <v>2</v>
@@ -2875,7 +2887,7 @@
       </c>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9">
       <c r="A74" s="2">
         <v>45826</v>
       </c>
@@ -2902,7 +2914,7 @@
       </c>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9">
       <c r="A75" s="9">
         <v>45826</v>
       </c>
@@ -2929,7 +2941,7 @@
       </c>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9">
       <c r="A76" s="2">
         <v>45826</v>
       </c>
@@ -2956,7 +2968,7 @@
       </c>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9">
       <c r="A77" s="9">
         <v>45826</v>
       </c>
@@ -2983,7 +2995,7 @@
       </c>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9">
       <c r="A78" s="2">
         <v>45826</v>
       </c>
@@ -3010,7 +3022,7 @@
       </c>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9">
       <c r="A79" s="9">
         <v>45826</v>
       </c>
@@ -3037,7 +3049,7 @@
       </c>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9">
       <c r="A80" s="2">
         <v>45826</v>
       </c>
@@ -3064,7 +3076,7 @@
       </c>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9">
       <c r="A81" s="9">
         <v>45826</v>
       </c>
@@ -3091,7 +3103,7 @@
       </c>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9">
       <c r="A82" s="2">
         <v>45826</v>
       </c>
@@ -3118,7 +3130,7 @@
       </c>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9">
       <c r="A83" s="9">
         <v>45826</v>
       </c>
@@ -3145,7 +3157,7 @@
       </c>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9">
       <c r="A84" s="2">
         <v>45826</v>
       </c>
@@ -3172,7 +3184,7 @@
       </c>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9">
       <c r="A85" s="9">
         <v>45826</v>
       </c>
@@ -3199,7 +3211,7 @@
       </c>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9">
       <c r="A86" s="2">
         <v>45826</v>
       </c>
@@ -3226,7 +3238,7 @@
       </c>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9">
       <c r="A87" s="9">
         <v>45826</v>
       </c>
@@ -3253,7 +3265,7 @@
       </c>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9">
       <c r="A88" s="2">
         <v>45826</v>
       </c>
@@ -3261,7 +3273,7 @@
         <v>18</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D88" s="3">
         <v>3</v>
@@ -3280,7 +3292,7 @@
       </c>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9">
       <c r="A89" s="9">
         <v>45826</v>
       </c>
@@ -3288,7 +3300,7 @@
         <v>18</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D89" s="5">
         <v>3</v>
@@ -3307,7 +3319,7 @@
       </c>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9">
       <c r="A90" s="2">
         <v>45826</v>
       </c>
@@ -3334,7 +3346,7 @@
       </c>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9">
       <c r="A91" s="9">
         <v>45826</v>
       </c>
@@ -3361,7 +3373,7 @@
       </c>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9">
       <c r="A92" s="2">
         <v>45826</v>
       </c>
@@ -3388,7 +3400,7 @@
       </c>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9">
       <c r="A93" s="9">
         <v>45826</v>
       </c>
@@ -3415,7 +3427,7 @@
       </c>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9">
       <c r="A94" s="2">
         <v>45826</v>
       </c>
@@ -3442,7 +3454,7 @@
       </c>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9">
       <c r="A95" s="9">
         <v>45826</v>
       </c>
@@ -3469,7 +3481,7 @@
       </c>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9">
       <c r="A96" s="2">
         <v>45826</v>
       </c>
@@ -3496,7 +3508,7 @@
       </c>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9">
       <c r="A97" s="10">
         <v>45826</v>
       </c>
@@ -3523,28 +3535,28 @@
       </c>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9">
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9">
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9">
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9">
       <c r="I101" s="1"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9">
       <c r="I102" s="1"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9">
       <c r="I103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9">
       <c r="I104" s="1"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9">
       <c r="I105" s="1"/>
     </row>
   </sheetData>

</xml_diff>